<commit_message>
fixed perubahan besar pada nomenklatur
</commit_message>
<xml_diff>
--- a/public/template/template_impor_kegiatan.xlsx
+++ b/public/template/template_impor_kegiatan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\emonev\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0B5AC5-BA99-4B12-A061-B74A3D973BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1992AF09-5B92-4EBE-A01E-0CFB09BDC6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{92DF29B1-657A-46F2-A1D7-C0F51ECE3890}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>No</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>Tahun Perubahan</t>
+  </si>
+  <si>
+    <t>Kode Urusan</t>
+  </si>
+  <si>
+    <t>Kode Program</t>
   </si>
 </sst>
 </file>
@@ -405,38 +411,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E01D98B-E692-4B6F-ACA2-254A33EABCFE}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.5546875" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.5546875" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>